<commit_message>
ima sitnih dorada u kodu, sa novim rezultatima
</commit_message>
<xml_diff>
--- a/klasa1direktno.xlsx
+++ b/klasa1direktno.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Kamera gleda direktno u marker:</t>
   </si>
@@ -28,24 +28,12 @@
     <t>Greska po y</t>
   </si>
   <si>
-    <t>Greska po z</t>
-  </si>
-  <si>
     <t>Euklidsko rastojanje greske</t>
   </si>
   <si>
     <t>fail</t>
   </si>
   <si>
-    <t>Greska po x*</t>
-  </si>
-  <si>
-    <t>Greska po y*</t>
-  </si>
-  <si>
-    <t>Greska po z*</t>
-  </si>
-  <si>
     <t>Euklidsko rastojanje greske*</t>
   </si>
   <si>
@@ -53,6 +41,9 @@
   </si>
   <si>
     <t>Marker detektovan na 4 slike</t>
+  </si>
+  <si>
+    <t>Greska po z* (yaw)</t>
   </si>
 </sst>
 </file>
@@ -88,7 +79,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -169,17 +160,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,37 +498,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,200 +537,152 @@
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>20.6235</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>30.4192</v>
       </c>
       <c r="C9" s="5">
-        <v>2.5225200000000001</v>
+        <v>2.6663999999999999</v>
       </c>
       <c r="D9" s="5">
-        <v>0.62199400000000005</v>
+        <v>0.82738400000000001</v>
       </c>
       <c r="E9" s="5">
-        <v>0.73248500000000005</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2.69936</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.79182</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>45.2806</v>
       </c>
       <c r="C10" s="5">
-        <v>7.6842699999999997</v>
+        <v>4.8058199999999998</v>
       </c>
       <c r="D10" s="5">
-        <v>2.4074499999999999</v>
+        <v>1.4963900000000001</v>
       </c>
       <c r="E10" s="5">
-        <v>13.337</v>
-      </c>
-      <c r="F10" s="5">
-        <v>15.579499999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5.0333899999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>60.210700000000003</v>
       </c>
       <c r="C11" s="5">
-        <v>10.242900000000001</v>
+        <v>14.548500000000001</v>
       </c>
       <c r="D11" s="5">
-        <v>3.81616</v>
+        <v>3.9600200000000001</v>
       </c>
       <c r="E11" s="5">
-        <v>17.580200000000001</v>
-      </c>
-      <c r="F11" s="5">
-        <v>20.7013</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>15.0778</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>75.168700000000001</v>
       </c>
       <c r="C12" s="5">
-        <v>12.4755</v>
+        <v>12.3508</v>
       </c>
       <c r="D12" s="5">
-        <v>4.6388400000000001</v>
+        <v>2.8748900000000002</v>
       </c>
       <c r="E12" s="5">
-        <v>9.2496299999999998</v>
-      </c>
-      <c r="F12" s="5">
-        <v>16.208400000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12.680999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>20.6235</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>30.4192</v>
       </c>
       <c r="C16" s="5">
-        <v>3.9872100000000001</v>
+        <v>4.0833899999999996</v>
       </c>
       <c r="D16" s="5">
-        <v>0.7389</v>
-      </c>
-      <c r="E16" s="5">
-        <v>3.83447</v>
-      </c>
-      <c r="F16" s="5">
-        <v>5.58094</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>4.0833899999999996</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>45.2806</v>
       </c>
       <c r="C17" s="5">
-        <v>19.500800000000002</v>
+        <v>5.7104699999999999</v>
       </c>
       <c r="D17" s="5">
-        <v>0.79059400000000002</v>
-      </c>
-      <c r="E17" s="5">
-        <v>10.719799999999999</v>
-      </c>
-      <c r="F17" s="5">
-        <v>22.267099999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5.7104699999999999</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>60.210700000000003</v>
       </c>
       <c r="C18" s="5">
-        <v>20.133800000000001</v>
+        <v>15.342000000000001</v>
       </c>
       <c r="D18" s="5">
-        <v>0.60498600000000002</v>
-      </c>
-      <c r="E18" s="5">
-        <v>11.2806</v>
-      </c>
-      <c r="F18" s="5">
-        <v>23.086500000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>15.342000000000001</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>75.168700000000001</v>
       </c>
       <c r="C19" s="5">
-        <v>5.1137699999999997</v>
+        <v>9.0066299999999995</v>
       </c>
       <c r="D19" s="5">
-        <v>0.83673500000000001</v>
-      </c>
-      <c r="E19" s="5">
-        <v>9.3217800000000004</v>
-      </c>
-      <c r="F19" s="5">
-        <v>10.6652</v>
-      </c>
+        <v>9.0066299999999995</v>
+      </c>
+      <c r="E19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>